<commit_message>
TICC-239; Updated 0037 RegExp
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Participant identifier schemes v8.3.xlsx
+++ b/work-in-progress/Peppol Code Lists - Participant identifier schemes v8.3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\peppol-edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD31574-BDC1-4985-9B91-E3FA6F672A79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A25B80A-9716-4AB2-A0E7-1E1DB6A87A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2205" yWindow="1110" windowWidth="26340" windowHeight="16320" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23925" yWindow="1305" windowWidth="26340" windowHeight="16320" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Participant Identifier Scheme" sheetId="1" r:id="rId1"/>
@@ -1506,10 +1506,6 @@
     <t>RegEx: [0-9]{14}</t>
   </si>
   <si>
-    <t>RegEx: 0037[0-9]{8}[0-9A-Z]{0,5}
-Check Digit: mod11 of 8-digit OrgCode (weights 2, 4, 8, 5, 10, 9, 7 [right to left] or 7, 9, 10, 5, 8, 4, 2, 1 [left to right])</t>
-  </si>
-  <si>
     <t>RegEx: [0-9]{9}</t>
   </si>
   <si>
@@ -1876,6 +1872,10 @@
   </si>
   <si>
     <t>8.3</t>
+  </si>
+  <si>
+    <t>RegEx: (0037)?[0-9]{7}-?[0-9][0-9A-Z]{0,5}
+Check Digit: mod11 of 8-digit OrgCode (weights 2, 4, 8, 5, 10, 9, 7 [right to left] or 7, 9, 10, 5, 8, 4, 2, 1 [left to right])</t>
   </si>
 </sst>
 </file>
@@ -2671,10 +2671,10 @@
   <dimension ref="A1:AMN98"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D86" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A93" sqref="A93"/>
+      <selection pane="bottomRight" activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2713,16 +2713,16 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>492</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>500</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>493</v>
-      </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>501</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>502</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>5</v>
@@ -2760,7 +2760,7 @@
         <v>13</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>366</v>
@@ -2798,7 +2798,7 @@
         <v>13</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J3" s="9" t="s">
         <v>367</v>
@@ -2833,7 +2833,7 @@
         <v>25</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J4" s="9" t="s">
         <v>368</v>
@@ -2868,7 +2868,7 @@
         <v>13</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>369</v>
@@ -2880,7 +2880,7 @@
         <v>390</v>
       </c>
       <c r="M5" s="10" t="s">
-        <v>434</v>
+        <v>529</v>
       </c>
       <c r="N5" s="7" t="s">
         <v>402</v>
@@ -2906,7 +2906,7 @@
         <v>13</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J6" s="9" t="s">
         <v>370</v>
@@ -2918,7 +2918,7 @@
         <v>391</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="N6" s="7" t="s">
         <v>403</v>
@@ -2944,7 +2944,7 @@
         <v>13</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J7" s="9" t="s">
         <v>48</v>
@@ -2956,7 +2956,7 @@
         <v>392</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="N7" s="7" t="s">
         <v>404</v>
@@ -2982,7 +2982,7 @@
         <v>13</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J8" s="9" t="s">
         <v>371</v>
@@ -2991,7 +2991,7 @@
         <v>32</v>
       </c>
       <c r="M8" s="10" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="180" x14ac:dyDescent="0.25">
@@ -3014,7 +3014,7 @@
         <v>13</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J9" s="9" t="s">
         <v>372</v>
@@ -3023,7 +3023,7 @@
         <v>32</v>
       </c>
       <c r="M9" s="10" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N9" s="7" t="s">
         <v>405</v>
@@ -3049,7 +3049,7 @@
         <v>58</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J10" s="9" t="s">
         <v>373</v>
@@ -3058,7 +3058,7 @@
         <v>32</v>
       </c>
       <c r="M10" s="10" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N10" s="7" t="s">
         <v>406</v>
@@ -3084,7 +3084,7 @@
         <v>63</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J11" s="9" t="s">
         <v>64</v>
@@ -3116,7 +3116,7 @@
         <v>13</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J12" s="9" t="s">
         <v>73</v>
@@ -3148,7 +3148,7 @@
         <v>13</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J13" s="9" t="s">
         <v>127</v>
@@ -3180,7 +3180,7 @@
         <v>79</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J14" s="9" t="s">
         <v>374</v>
@@ -3192,7 +3192,7 @@
         <v>393</v>
       </c>
       <c r="M14" s="10" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="N14" s="7" t="s">
         <v>409</v>
@@ -3218,7 +3218,7 @@
         <v>79</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J15" s="9" t="s">
         <v>339</v>
@@ -3227,7 +3227,7 @@
         <v>338</v>
       </c>
       <c r="M15" s="10" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="N15" s="7" t="s">
         <v>342</v>
@@ -3253,7 +3253,7 @@
         <v>84</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J16" s="9" t="s">
         <v>375</v>
@@ -3262,33 +3262,33 @@
         <v>383</v>
       </c>
       <c r="M16" s="10" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="17" spans="1:14 1028:1028" ht="150" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
+        <v>504</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>505</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="C17" s="7" t="s">
+        <v>502</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>506</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="E17" s="7" t="s">
+        <v>507</v>
+      </c>
+      <c r="F17" s="8" t="s">
         <v>503</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>507</v>
-      </c>
-      <c r="E17" s="7" t="s">
+      <c r="G17" s="10" t="s">
+        <v>493</v>
+      </c>
+      <c r="J17" s="9" t="s">
         <v>508</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>504</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>494</v>
-      </c>
-      <c r="J17" s="9" t="s">
-        <v>509</v>
       </c>
       <c r="K17" s="9" t="s">
         <v>32</v>
@@ -3314,7 +3314,7 @@
         <v>89</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J18" s="9" t="s">
         <v>376</v>
@@ -3326,7 +3326,7 @@
         <v>394</v>
       </c>
       <c r="M18" s="10" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="N18" s="7" t="s">
         <v>410</v>
@@ -3352,7 +3352,7 @@
         <v>89</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J19" s="9" t="s">
         <v>377</v>
@@ -3364,7 +3364,7 @@
         <v>395</v>
       </c>
       <c r="M19" s="10" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="N19" s="7" t="s">
         <v>411</v>
@@ -3390,7 +3390,7 @@
         <v>89</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J20" s="9" t="s">
         <v>100</v>
@@ -3402,7 +3402,7 @@
         <v>396</v>
       </c>
       <c r="M20" s="10" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="21" spans="1:14 1028:1028" ht="45" x14ac:dyDescent="0.25">
@@ -3425,7 +3425,7 @@
         <v>106</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J21" s="9" t="s">
         <v>107</v>
@@ -3434,7 +3434,7 @@
         <v>32</v>
       </c>
       <c r="M21" s="10" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="22" spans="1:14 1028:1028" ht="105" x14ac:dyDescent="0.25">
@@ -3457,7 +3457,7 @@
         <v>63</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J22" s="9" t="s">
         <v>378</v>
@@ -3466,7 +3466,7 @@
         <v>385</v>
       </c>
       <c r="M22" s="10" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="N22" s="7" t="s">
         <v>412</v>
@@ -3492,7 +3492,7 @@
         <v>63</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J23" s="9" t="s">
         <v>379</v>
@@ -3501,7 +3501,7 @@
         <v>386</v>
       </c>
       <c r="M23" s="10" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="24" spans="1:14 1028:1028" ht="45" x14ac:dyDescent="0.25">
@@ -3524,7 +3524,7 @@
         <v>79</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J24" s="9" t="s">
         <v>348</v>
@@ -3533,7 +3533,7 @@
         <v>349</v>
       </c>
       <c r="M24" s="10" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="25" spans="1:14 1028:1028" ht="409.5" x14ac:dyDescent="0.25">
@@ -3556,7 +3556,7 @@
         <v>79</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J25" s="9" t="s">
         <v>380</v>
@@ -3565,7 +3565,7 @@
         <v>353</v>
       </c>
       <c r="M25" s="10" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="26" spans="1:14 1028:1028" ht="90" x14ac:dyDescent="0.25">
@@ -3588,7 +3588,7 @@
         <v>79</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J26" s="9" t="s">
         <v>123</v>
@@ -3600,7 +3600,7 @@
         <v>397</v>
       </c>
       <c r="M26" s="10" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="27" spans="1:14 1028:1028" ht="30" x14ac:dyDescent="0.25">
@@ -3623,7 +3623,7 @@
         <v>359</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J27" s="9" t="s">
         <v>360</v>
@@ -3633,7 +3633,7 @@
       </c>
       <c r="L27" s="11"/>
       <c r="M27" s="11" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="N27" s="7" t="s">
         <v>361</v>
@@ -3651,7 +3651,7 @@
         <v>226</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>364</v>
@@ -3660,20 +3660,20 @@
         <v>359</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J28" s="9" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="K28" s="9" t="s">
         <v>365</v>
       </c>
       <c r="L28" s="11"/>
       <c r="M28" s="11" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="N28" s="7" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="AMN28" s="7"/>
     </row>
@@ -3697,257 +3697,257 @@
         <v>426</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J29" s="9" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="K29" s="9" t="s">
         <v>427</v>
       </c>
       <c r="L29" s="11"/>
       <c r="M29" s="10" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="AMN29" s="7"/>
     </row>
     <row r="30" spans="1:14 1028:1028" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D30" s="7" t="s">
+        <v>465</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>464</v>
+      </c>
+      <c r="F30" s="12" t="s">
         <v>466</v>
       </c>
-      <c r="E30" s="7" t="s">
-        <v>465</v>
-      </c>
-      <c r="F30" s="12" t="s">
+      <c r="G30" s="10" t="s">
+        <v>493</v>
+      </c>
+      <c r="J30" s="9" t="s">
         <v>467</v>
-      </c>
-      <c r="G30" s="10" t="s">
-        <v>494</v>
-      </c>
-      <c r="J30" s="9" t="s">
-        <v>468</v>
       </c>
       <c r="K30" s="9" t="s">
         <v>32</v>
       </c>
       <c r="L30" s="11" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="M30" s="10" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="AMN30" s="7"/>
     </row>
     <row r="31" spans="1:14 1028:1028" ht="255" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>51</v>
       </c>
       <c r="D31" s="7" t="s">
+        <v>472</v>
+      </c>
+      <c r="E31" s="7" t="s">
         <v>473</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="F31" s="12" t="s">
+        <v>466</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>493</v>
+      </c>
+      <c r="J31" s="9" t="s">
         <v>474</v>
-      </c>
-      <c r="F31" s="12" t="s">
-        <v>467</v>
-      </c>
-      <c r="G31" s="10" t="s">
-        <v>494</v>
-      </c>
-      <c r="J31" s="9" t="s">
-        <v>475</v>
       </c>
       <c r="L31" s="11"/>
       <c r="M31" s="10" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="AMN31" s="7"/>
     </row>
     <row r="32" spans="1:14 1028:1028" ht="105" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>51</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J32" s="9" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="L32" s="11"/>
       <c r="M32" s="10" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="AMN32" s="7"/>
     </row>
     <row r="33" spans="1:14 1028:1028" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
+        <v>477</v>
+      </c>
+      <c r="B33" s="7" t="s">
         <v>478</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>479</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D33" s="7" t="s">
+        <v>481</v>
+      </c>
+      <c r="E33" s="7" t="s">
         <v>482</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="F33" s="12" t="s">
+        <v>466</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>493</v>
+      </c>
+      <c r="J33" s="9" t="s">
         <v>483</v>
       </c>
-      <c r="F33" s="12" t="s">
-        <v>467</v>
-      </c>
-      <c r="G33" s="10" t="s">
-        <v>494</v>
-      </c>
-      <c r="J33" s="9" t="s">
+      <c r="K33" s="9" t="s">
         <v>484</v>
-      </c>
-      <c r="K33" s="9" t="s">
-        <v>485</v>
       </c>
       <c r="L33" s="11"/>
       <c r="M33" s="10" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="AMN33" s="7"/>
     </row>
     <row r="34" spans="1:14 1028:1028" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="B34" s="7" t="s">
         <v>480</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>481</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D34" s="7" t="s">
+        <v>486</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>482</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>466</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>493</v>
+      </c>
+      <c r="J34" s="9" t="s">
         <v>487</v>
       </c>
-      <c r="E34" s="7" t="s">
-        <v>483</v>
-      </c>
-      <c r="F34" s="12" t="s">
-        <v>467</v>
-      </c>
-      <c r="G34" s="10" t="s">
-        <v>494</v>
-      </c>
-      <c r="J34" s="9" t="s">
+      <c r="K34" s="9" t="s">
         <v>488</v>
-      </c>
-      <c r="K34" s="9" t="s">
-        <v>489</v>
       </c>
       <c r="L34" s="11"/>
       <c r="M34" s="10" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="AMN34" s="7"/>
     </row>
     <row r="35" spans="1:14 1028:1028" ht="150" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
+        <v>509</v>
+      </c>
+      <c r="B35" s="7" t="s">
         <v>510</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>511</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D35" s="7" t="s">
+        <v>511</v>
+      </c>
+      <c r="E35" s="7" t="s">
         <v>512</v>
       </c>
-      <c r="E35" s="7" t="s">
+      <c r="F35" s="12" t="s">
+        <v>503</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>493</v>
+      </c>
+      <c r="J35" s="9" t="s">
         <v>513</v>
-      </c>
-      <c r="F35" s="12" t="s">
-        <v>504</v>
-      </c>
-      <c r="G35" s="10" t="s">
-        <v>494</v>
-      </c>
-      <c r="J35" s="9" t="s">
-        <v>514</v>
       </c>
       <c r="K35" s="9" t="s">
         <v>32</v>
       </c>
       <c r="L35" s="11"/>
       <c r="M35" s="10" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="N35" s="7" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="AMN35" s="7"/>
     </row>
     <row r="36" spans="1:14 1028:1028" ht="240" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
+        <v>516</v>
+      </c>
+      <c r="B36" s="7" t="s">
         <v>517</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>518</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D36" s="7" t="s">
+        <v>518</v>
+      </c>
+      <c r="E36" s="7" t="s">
         <v>519</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="F36" s="12" t="s">
+        <v>503</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>493</v>
+      </c>
+      <c r="J36" s="9" t="s">
         <v>520</v>
-      </c>
-      <c r="F36" s="12" t="s">
-        <v>504</v>
-      </c>
-      <c r="G36" s="10" t="s">
-        <v>494</v>
-      </c>
-      <c r="J36" s="9" t="s">
-        <v>521</v>
       </c>
       <c r="K36" s="9" t="s">
         <v>32</v>
       </c>
       <c r="L36" s="11"/>
       <c r="M36" s="10" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="N36" s="7" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="AMN36" s="7"/>
     </row>
@@ -3971,7 +3971,7 @@
         <v>13</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J37" s="9" t="s">
         <v>127</v>
@@ -4003,13 +4003,13 @@
         <v>13</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="L38" s="10" t="s">
         <v>398</v>
       </c>
       <c r="M38" s="10" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="39" spans="1:14 1028:1028" ht="45" x14ac:dyDescent="0.25">
@@ -4032,13 +4032,13 @@
         <v>13</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="L39" s="10" t="s">
         <v>134</v>
       </c>
       <c r="M39" s="10" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="40" spans="1:14 1028:1028" ht="45" x14ac:dyDescent="0.25">
@@ -4061,7 +4061,7 @@
         <v>13</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="L40" s="10" t="s">
         <v>134</v>
@@ -4087,19 +4087,19 @@
         <v>13</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="J41" s="9" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="L41" s="10" t="s">
         <v>141</v>
       </c>
       <c r="M41" s="10" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="42" spans="1:14 1028:1028" ht="285" x14ac:dyDescent="0.25">
@@ -4122,16 +4122,16 @@
         <v>13</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="L42" s="10" t="s">
         <v>399</v>
       </c>
       <c r="M42" s="10" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="N42" s="7" t="s">
         <v>415</v>
@@ -4157,13 +4157,13 @@
         <v>13</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J43" s="9" t="s">
         <v>100</v>
       </c>
       <c r="M43" s="10" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="N43" s="7" t="s">
         <v>416</v>
@@ -4189,7 +4189,7 @@
         <v>13</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="H44" s="8" t="s">
         <v>150</v>
@@ -4198,7 +4198,7 @@
         <v>155</v>
       </c>
       <c r="M44" s="10" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="N44" s="7" t="s">
         <v>417</v>
@@ -4221,10 +4221,10 @@
         <v>13</v>
       </c>
       <c r="G45" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="M45" s="10" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="46" spans="1:14 1028:1028" ht="75" x14ac:dyDescent="0.25">
@@ -4245,7 +4245,7 @@
         <v>13</v>
       </c>
       <c r="G46" s="10" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="H46" s="8" t="s">
         <v>150</v>
@@ -4254,10 +4254,10 @@
         <v>159</v>
       </c>
       <c r="M46" s="10" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="N46" s="7" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="47" spans="1:14 1028:1028" x14ac:dyDescent="0.25">
@@ -4280,7 +4280,7 @@
         <v>13</v>
       </c>
       <c r="G47" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="N47" s="7" t="s">
         <v>418</v>
@@ -4303,7 +4303,7 @@
         <v>13</v>
       </c>
       <c r="G48" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="L48" s="10" t="s">
         <v>168</v>
@@ -4327,13 +4327,13 @@
         <v>13</v>
       </c>
       <c r="G49" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="L49" s="10" t="s">
         <v>400</v>
       </c>
       <c r="M49" s="10" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="N49" s="7" t="s">
         <v>419</v>
@@ -4356,7 +4356,7 @@
         <v>13</v>
       </c>
       <c r="G50" s="10" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="H50" s="8" t="s">
         <v>176</v>
@@ -4379,7 +4379,7 @@
         <v>13</v>
       </c>
       <c r="G51" s="10" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="H51" s="8" t="s">
         <v>63</v>
@@ -4391,7 +4391,7 @@
         <v>386</v>
       </c>
       <c r="M51" s="10" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="N51" s="7" t="s">
         <v>180</v>
@@ -4417,7 +4417,7 @@
         <v>183</v>
       </c>
       <c r="G52" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J52" s="9" t="s">
         <v>381</v>
@@ -4441,7 +4441,7 @@
         <v>176</v>
       </c>
       <c r="G53" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J53" s="9" t="s">
         <v>187</v>
@@ -4470,7 +4470,7 @@
         <v>176</v>
       </c>
       <c r="G54" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="55" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -4493,7 +4493,7 @@
         <v>150</v>
       </c>
       <c r="G55" s="10" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="H55" s="8" t="s">
         <v>359</v>
@@ -4520,7 +4520,7 @@
         <v>150</v>
       </c>
       <c r="G56" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
@@ -4541,7 +4541,7 @@
         <v>150</v>
       </c>
       <c r="G57" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
@@ -4562,7 +4562,7 @@
         <v>150</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
@@ -4583,7 +4583,7 @@
         <v>150</v>
       </c>
       <c r="G59" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
@@ -4604,7 +4604,7 @@
         <v>150</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
@@ -4625,7 +4625,7 @@
         <v>150</v>
       </c>
       <c r="G61" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
@@ -4645,7 +4645,7 @@
         <v>150</v>
       </c>
       <c r="G62" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
@@ -4666,7 +4666,7 @@
         <v>150</v>
       </c>
       <c r="G63" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
@@ -4687,7 +4687,7 @@
         <v>150</v>
       </c>
       <c r="G64" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -4708,7 +4708,7 @@
         <v>150</v>
       </c>
       <c r="G65" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -4729,7 +4729,7 @@
         <v>150</v>
       </c>
       <c r="G66" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -4750,7 +4750,7 @@
         <v>150</v>
       </c>
       <c r="G67" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -4771,7 +4771,7 @@
         <v>150</v>
       </c>
       <c r="G68" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -4792,7 +4792,7 @@
         <v>150</v>
       </c>
       <c r="G69" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -4813,7 +4813,7 @@
         <v>150</v>
       </c>
       <c r="G70" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -4834,7 +4834,7 @@
         <v>150</v>
       </c>
       <c r="G71" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -4855,7 +4855,7 @@
         <v>150</v>
       </c>
       <c r="G72" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -4876,7 +4876,7 @@
         <v>150</v>
       </c>
       <c r="G73" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -4897,7 +4897,7 @@
         <v>150</v>
       </c>
       <c r="G74" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -4918,7 +4918,7 @@
         <v>150</v>
       </c>
       <c r="G75" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4939,7 +4939,7 @@
         <v>150</v>
       </c>
       <c r="G76" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -4960,7 +4960,7 @@
         <v>150</v>
       </c>
       <c r="G77" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -4981,7 +4981,7 @@
         <v>150</v>
       </c>
       <c r="G78" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -5002,7 +5002,7 @@
         <v>150</v>
       </c>
       <c r="G79" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -5023,7 +5023,7 @@
         <v>150</v>
       </c>
       <c r="G80" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.25">
@@ -5044,7 +5044,7 @@
         <v>150</v>
       </c>
       <c r="G81" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="I81" s="3"/>
     </row>
@@ -5066,7 +5066,7 @@
         <v>150</v>
       </c>
       <c r="G82" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="I82" s="3"/>
     </row>
@@ -5088,7 +5088,7 @@
         <v>150</v>
       </c>
       <c r="G83" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="I83" s="3"/>
     </row>
@@ -5110,7 +5110,7 @@
         <v>150</v>
       </c>
       <c r="G84" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.25">
@@ -5130,7 +5130,7 @@
         <v>150</v>
       </c>
       <c r="G85" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.25">
@@ -5151,7 +5151,7 @@
         <v>150</v>
       </c>
       <c r="G86" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="I86" s="4"/>
     </row>
@@ -5173,7 +5173,7 @@
         <v>150</v>
       </c>
       <c r="G87" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.25">
@@ -5193,7 +5193,7 @@
         <v>320</v>
       </c>
       <c r="G88" s="10" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="H88" s="8" t="s">
         <v>89</v>
@@ -5220,7 +5220,7 @@
         <v>325</v>
       </c>
       <c r="G89" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="I89" s="3"/>
     </row>
@@ -5244,10 +5244,10 @@
         <v>84</v>
       </c>
       <c r="G90" s="10" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="H90" s="8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="I90" s="3"/>
       <c r="J90" s="9" t="s">
@@ -5257,7 +5257,7 @@
         <v>401</v>
       </c>
       <c r="M90" s="10" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.25">
@@ -5277,7 +5277,7 @@
         <v>84</v>
       </c>
       <c r="G91" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.25">
@@ -5291,13 +5291,13 @@
         <v>226</v>
       </c>
       <c r="D92" s="7" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F92" s="8" t="s">
         <v>106</v>
       </c>
       <c r="G92" s="10" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="H92" s="8" t="s">
         <v>359</v>
@@ -5309,22 +5309,22 @@
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
+        <v>523</v>
+      </c>
+      <c r="B93" s="7" t="s">
         <v>524</v>
       </c>
-      <c r="B93" s="7" t="s">
+      <c r="C93" s="7" t="s">
         <v>525</v>
       </c>
-      <c r="C93" s="7" t="s">
+      <c r="D93" s="7" t="s">
         <v>526</v>
       </c>
-      <c r="D93" s="7" t="s">
-        <v>527</v>
-      </c>
       <c r="F93" s="8" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="G93" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="98" spans="9:9" x14ac:dyDescent="0.25">

</xml_diff>